<commit_message>
SAS Advance Cheat Sheet
</commit_message>
<xml_diff>
--- a/Advance/Cheat_sheet.xlsx
+++ b/Advance/Cheat_sheet.xlsx
@@ -700,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -828,7 +828,7 @@
         <v>78</v>
       </c>
       <c r="C11" s="10">
-        <v>42914</v>
+        <v>42918</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
         <v>79</v>
       </c>
       <c r="C12" s="10">
-        <v>42915</v>
+        <v>42918</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -850,7 +850,7 @@
         <v>80</v>
       </c>
       <c r="C13" s="10">
-        <v>42916</v>
+        <v>42918</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>